<commit_message>
基于 total.js bower grunt 的工程框架
</commit_message>
<xml_diff>
--- a/B01/t01.xlsx
+++ b/B01/t01.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="3"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="310">
   <si>
     <t>Version</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1071,12 +1071,28 @@
     <t>系统常量配置表</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
+  <si>
+    <t>渠道类型名称</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>渠道类型编码</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>渠道类型</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="16">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1346,7 +1362,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="常规 3" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1360,7 +1376,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1434,6 +1450,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1468,6 +1485,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1643,14 +1661,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21:G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.625" style="2" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="16.625" style="2" customWidth="1" collapsed="1"/>
@@ -1664,7 +1682,7 @@
     <col min="10" max="16384" width="9" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1682,7 +1700,7 @@
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1700,7 +1718,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1718,7 +1736,7 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1736,7 +1754,7 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1754,7 +1772,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1772,7 +1790,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1790,7 +1808,7 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1808,7 +1826,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" ht="15.75">
+    <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1826,7 +1844,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" ht="23.25">
+    <row r="10" spans="1:16" ht="23.25" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="32" t="s">
         <v>71</v>
@@ -1846,7 +1864,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" ht="23.25">
+    <row r="11" spans="1:16" ht="23.25" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1864,7 +1882,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" ht="15.75">
+    <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="6" t="s">
         <v>0</v>
@@ -1894,7 +1912,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" ht="15.75">
+    <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -1912,7 +1930,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" ht="15.75">
+    <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1930,7 +1948,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" ht="15.75">
+    <row r="15" spans="1:16" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -1948,7 +1966,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" ht="15.75">
+    <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1966,7 +1984,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" ht="15.75">
+    <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1984,7 +2002,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" ht="15.75">
+    <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -2002,7 +2020,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" ht="15.75">
+    <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -2020,7 +2038,7 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="1:16" ht="15.75">
+    <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
@@ -2038,7 +2056,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" ht="15.75">
+    <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="33" t="s">
         <v>72</v>
@@ -2058,7 +2076,7 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="1:16" ht="15.75">
+    <row r="22" spans="1:16" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="31" t="s">
         <v>6</v>
@@ -2078,7 +2096,7 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
       <c r="B23" s="31" t="s">
         <v>7</v>
@@ -2098,7 +2116,7 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
       <c r="B24" s="31" t="s">
         <v>8</v>
@@ -2118,7 +2136,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
       <c r="B25" s="31" t="s">
         <v>9</v>
@@ -2138,7 +2156,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16" ht="14.25">
+    <row r="26" spans="1:16" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
       <c r="B26" s="30" t="s">
         <v>10</v>
@@ -2158,7 +2176,7 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A27" s="1"/>
       <c r="B27" s="31" t="s">
         <v>11</v>
@@ -2178,7 +2196,7 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2196,7 +2214,7 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2214,7 +2232,7 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2232,7 +2250,7 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2250,7 +2268,7 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2268,7 +2286,7 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2286,7 +2304,7 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2304,7 +2322,7 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2322,7 +2340,7 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2340,7 +2358,7 @@
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2358,7 +2376,7 @@
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2376,7 +2394,7 @@
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2394,7 +2412,7 @@
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2412,7 +2430,7 @@
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2430,7 +2448,7 @@
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2448,7 +2466,7 @@
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2466,7 +2484,7 @@
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2484,7 +2502,7 @@
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2502,7 +2520,7 @@
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -2520,7 +2538,7 @@
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2538,7 +2556,7 @@
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2556,7 +2574,7 @@
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2574,7 +2592,7 @@
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2592,7 +2610,7 @@
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2628,14 +2646,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.125" style="16" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="17.375" style="16" customWidth="1" collapsed="1"/>
@@ -2643,14 +2661,14 @@
     <col min="4" max="16384" width="9.125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5">
+    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
     </row>
-    <row r="2" spans="1:3" ht="16.5">
+    <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A2" s="17" t="s">
         <v>13</v>
       </c>
@@ -2661,7 +2679,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.5">
+    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A3" s="18" t="s">
         <v>16</v>
       </c>
@@ -2672,7 +2690,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5">
+    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -2683,7 +2701,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16.5">
+    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A5" s="18" t="s">
         <v>16</v>
       </c>
@@ -2694,7 +2712,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16.5">
+    <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A6" s="18" t="s">
         <v>16</v>
       </c>
@@ -2705,7 +2723,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="19" customFormat="1" ht="16.5">
+    <row r="7" spans="1:3" s="19" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A7" s="18" t="s">
         <v>16</v>
       </c>
@@ -2716,7 +2734,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="19" customFormat="1" ht="16.5">
+    <row r="8" spans="1:3" s="19" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A8" s="18" t="s">
         <v>16</v>
       </c>
@@ -2727,7 +2745,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="19" customFormat="1" ht="16.5">
+    <row r="9" spans="1:3" s="19" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
         <v>82</v>
       </c>
@@ -2738,7 +2756,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="19" customFormat="1" ht="16.5">
+    <row r="10" spans="1:3" s="19" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A10" s="18" t="s">
         <v>82</v>
       </c>
@@ -2749,7 +2767,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.5">
+    <row r="11" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A11" s="18" t="s">
         <v>25</v>
       </c>
@@ -2760,7 +2778,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16.5">
+    <row r="12" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A12" s="18" t="s">
         <v>25</v>
       </c>
@@ -2771,7 +2789,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16.5">
+    <row r="13" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A13" s="18" t="s">
         <v>25</v>
       </c>
@@ -2782,7 +2800,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16.5">
+    <row r="14" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A14" s="18" t="s">
         <v>25</v>
       </c>
@@ -2793,7 +2811,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16.5">
+    <row r="15" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A15" s="18" t="s">
         <v>25</v>
       </c>
@@ -2804,7 +2822,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16.5">
+    <row r="16" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A16" s="18" t="s">
         <v>25</v>
       </c>
@@ -2815,7 +2833,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16.5">
+    <row r="17" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A17" s="18" t="s">
         <v>25</v>
       </c>
@@ -2826,7 +2844,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16.5">
+    <row r="18" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A18" s="18" t="s">
         <v>25</v>
       </c>
@@ -2837,7 +2855,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16.5">
+    <row r="19" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A19" s="18" t="s">
         <v>25</v>
       </c>
@@ -2848,7 +2866,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16.5">
+    <row r="20" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A20" s="18" t="s">
         <v>25</v>
       </c>
@@ -2859,7 +2877,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16.5">
+    <row r="21" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A21" s="18" t="s">
         <v>25</v>
       </c>
@@ -2870,7 +2888,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="16.5">
+    <row r="22" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A22" s="18" t="s">
         <v>25</v>
       </c>
@@ -2881,7 +2899,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="33">
+    <row r="23" spans="1:3" ht="33" x14ac:dyDescent="0.15">
       <c r="A23" s="18" t="s">
         <v>25</v>
       </c>
@@ -2892,7 +2910,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="16.5">
+    <row r="24" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A24" s="18" t="s">
         <v>25</v>
       </c>
@@ -2903,7 +2921,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16.5">
+    <row r="25" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A25" s="18" t="s">
         <v>25</v>
       </c>
@@ -2921,14 +2939,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.875" style="23" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="16" style="23" bestFit="1" customWidth="1" collapsed="1"/>
@@ -2942,7 +2960,7 @@
     <col min="18" max="16384" width="9" style="22" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="20" t="s">
         <v>52</v>
       </c>
@@ -2968,7 +2986,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
         <v>76</v>
       </c>
@@ -2991,7 +3009,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="23" t="s">
         <v>76</v>
       </c>
@@ -3008,7 +3026,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="23" t="s">
         <v>76</v>
       </c>
@@ -3025,7 +3043,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
         <v>76</v>
       </c>
@@ -3048,7 +3066,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="23" t="s">
         <v>76</v>
       </c>
@@ -3071,7 +3089,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="23" t="s">
         <v>76</v>
       </c>
@@ -3094,7 +3112,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="23" t="s">
         <v>76</v>
       </c>
@@ -3117,7 +3135,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>76</v>
       </c>
@@ -3134,7 +3152,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="23" t="s">
         <v>76</v>
       </c>
@@ -3154,7 +3172,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="23" t="s">
         <v>76</v>
       </c>
@@ -3174,7 +3192,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="23" t="s">
         <v>76</v>
       </c>
@@ -3194,7 +3212,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="23" t="s">
         <v>76</v>
       </c>
@@ -3214,7 +3232,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="23" t="s">
         <v>76</v>
       </c>
@@ -3234,7 +3252,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="23" t="s">
         <v>76</v>
       </c>
@@ -3254,7 +3272,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="23" t="s">
         <v>76</v>
       </c>
@@ -3274,7 +3292,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="23" t="s">
         <v>76</v>
       </c>
@@ -3294,7 +3312,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="23" t="s">
         <v>76</v>
       </c>
@@ -3314,7 +3332,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="23" t="s">
         <v>76</v>
       </c>
@@ -3334,7 +3352,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="23" t="s">
         <v>76</v>
       </c>
@@ -3354,7 +3372,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="23" t="s">
         <v>76</v>
       </c>
@@ -3374,7 +3392,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="23" t="s">
         <v>76</v>
       </c>
@@ -3394,7 +3412,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="23" t="s">
         <v>76</v>
       </c>
@@ -3414,7 +3432,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="23" t="s">
         <v>76</v>
       </c>
@@ -3434,7 +3452,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="23" t="s">
         <v>76</v>
       </c>
@@ -3454,7 +3472,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="23" t="s">
         <v>76</v>
       </c>
@@ -3474,7 +3492,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="23" t="s">
         <v>76</v>
       </c>
@@ -3494,7 +3512,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="23" t="s">
         <v>76</v>
       </c>
@@ -3514,7 +3532,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="23" t="s">
         <v>76</v>
       </c>
@@ -3537,7 +3555,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="23" t="s">
         <v>76</v>
       </c>
@@ -3557,7 +3575,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="23" t="s">
         <v>76</v>
       </c>
@@ -3577,7 +3595,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="23" t="s">
         <v>76</v>
       </c>
@@ -3597,7 +3615,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="23" t="s">
         <v>76</v>
       </c>
@@ -3617,7 +3635,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="23" t="s">
         <v>76</v>
       </c>
@@ -3640,7 +3658,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
         <v>76</v>
       </c>
@@ -3663,7 +3681,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="23" t="s">
         <v>76</v>
       </c>
@@ -3689,7 +3707,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="23" t="s">
         <v>76</v>
       </c>
@@ -3709,7 +3727,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="23" t="s">
         <v>76</v>
       </c>
@@ -3729,7 +3747,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="23" t="s">
         <v>76</v>
       </c>
@@ -3749,7 +3767,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="23" t="s">
         <v>76</v>
       </c>
@@ -3769,7 +3787,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="23" t="s">
         <v>76</v>
       </c>
@@ -3789,7 +3807,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="23" t="s">
         <v>76</v>
       </c>
@@ -3809,7 +3827,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="23" t="s">
         <v>76</v>
       </c>
@@ -3829,7 +3847,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="23" t="s">
         <v>76</v>
       </c>
@@ -3849,7 +3867,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="23" t="s">
         <v>76</v>
       </c>
@@ -3869,7 +3887,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="23" t="s">
         <v>76</v>
       </c>
@@ -3889,7 +3907,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="23" t="s">
         <v>76</v>
       </c>
@@ -3909,7 +3927,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="23" t="s">
         <v>76</v>
       </c>
@@ -3929,7 +3947,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="23" t="s">
         <v>76</v>
       </c>
@@ -3949,7 +3967,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="23" t="s">
         <v>76</v>
       </c>
@@ -3966,7 +3984,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D51" s="23" t="s">
         <v>213</v>
       </c>
@@ -3974,7 +3992,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D52" s="23" t="s">
         <v>305</v>
       </c>
@@ -3994,16 +4012,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R141"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="G95" sqref="G95:G97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="10.25" style="23" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="21.875" style="23" bestFit="1" customWidth="1" collapsed="1"/>
@@ -4023,7 +4041,7 @@
     <col min="19" max="16384" width="9" style="22" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A1" s="20" t="s">
         <v>52</v>
       </c>
@@ -4073,7 +4091,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
         <v>76</v>
       </c>
@@ -4123,7 +4141,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="E3" s="29">
         <v>2</v>
       </c>
@@ -4149,12 +4167,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G4" s="23" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G5" s="23" t="s">
         <v>180</v>
       </c>
@@ -4162,37 +4180,37 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G6" s="23" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G7" s="23" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G8" s="23" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G9" s="23" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G10" s="23" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G11" s="23" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G12" s="23" t="s">
         <v>214</v>
       </c>
@@ -4200,22 +4218,22 @@
         <v>205</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G13" s="23" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G14" s="23" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G15" s="23" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G16" s="23" t="s">
         <v>213</v>
       </c>
@@ -4223,7 +4241,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G17" s="23" t="s">
         <v>204</v>
       </c>
@@ -4234,42 +4252,42 @@
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G18" s="23" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G19" s="23" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G20" s="23" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G21" s="23" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G22" s="23" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G23" s="23" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G24" s="23" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="23" t="s">
         <v>76</v>
       </c>
@@ -4310,7 +4328,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G26" s="23" t="s">
         <v>185</v>
       </c>
@@ -4327,17 +4345,17 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G27" s="23" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G28" s="23" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="23" t="s">
         <v>76</v>
       </c>
@@ -4378,7 +4396,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G30" s="23" t="s">
         <v>193</v>
       </c>
@@ -4395,17 +4413,17 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G31" s="23" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G32" s="23" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="23" t="s">
         <v>76</v>
       </c>
@@ -4437,132 +4455,132 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G34" s="23" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G35" s="23" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G36" s="23" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G37" s="23" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G38" s="23" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G39" s="23" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G40" s="23" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G41" s="23" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G42" s="23" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G43" s="23" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G44" s="23" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G45" s="23" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G46" s="23" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G47" s="23" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G48" s="23" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G49" s="23" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G50" s="23" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G51" s="23" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G52" s="23" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="53" spans="1:14">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G53" s="23" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G54" s="23" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G55" s="23" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G56" s="23" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G57" s="23" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G58" s="23" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A59" s="23" t="s">
         <v>76</v>
       </c>
@@ -4582,13 +4600,13 @@
         <v>177</v>
       </c>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D60" s="29"/>
       <c r="G60" s="23" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="61" spans="1:14">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D61" s="29"/>
       <c r="G61" s="23" t="s">
         <v>243</v>
@@ -4597,25 +4615,25 @@
         <v>205</v>
       </c>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D62" s="29"/>
       <c r="G62" s="23" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D63" s="29"/>
       <c r="G63" s="23" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D64" s="29"/>
       <c r="G64" s="23" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="65" spans="1:14">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A65" s="23" t="s">
         <v>76</v>
       </c>
@@ -4635,7 +4653,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="66" spans="1:14">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D66" s="29"/>
       <c r="G66" s="23" t="s">
         <v>248</v>
@@ -4644,19 +4662,19 @@
         <v>205</v>
       </c>
     </row>
-    <row r="67" spans="1:14">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D67" s="29"/>
       <c r="G67" s="23" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="68" spans="1:14">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D68" s="29"/>
       <c r="G68" s="23" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="69" spans="1:14">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A69" s="23" t="s">
         <v>76</v>
       </c>
@@ -4676,19 +4694,19 @@
         <v>251</v>
       </c>
     </row>
-    <row r="70" spans="1:14">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D70" s="29"/>
       <c r="G70" s="23" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="71" spans="1:14">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D71" s="29"/>
       <c r="G71" s="23" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="72" spans="1:14">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A72" s="23" t="s">
         <v>76</v>
       </c>
@@ -4708,22 +4726,22 @@
         <v>251</v>
       </c>
     </row>
-    <row r="73" spans="1:14">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G73" s="23" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="74" spans="1:14">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G74" s="23" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="75" spans="1:14">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G75" s="23" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="76" spans="1:14">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A76" s="23" t="s">
         <v>76</v>
       </c>
@@ -4740,7 +4758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:14">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A77" s="23" t="s">
         <v>76</v>
       </c>
@@ -4757,7 +4775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:14">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A78" s="23" t="s">
         <v>76</v>
       </c>
@@ -4774,7 +4792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:14">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A79" s="23" t="s">
         <v>76</v>
       </c>
@@ -4791,7 +4809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:14">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A80" s="23" t="s">
         <v>76</v>
       </c>
@@ -4808,7 +4826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="23" t="s">
         <v>76</v>
       </c>
@@ -4825,7 +4843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" s="23" t="s">
         <v>76</v>
       </c>
@@ -4842,7 +4860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="23" t="s">
         <v>76</v>
       </c>
@@ -4859,7 +4877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="23" t="s">
         <v>76</v>
       </c>
@@ -4876,7 +4894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="23" t="s">
         <v>76</v>
       </c>
@@ -4893,7 +4911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="23" t="s">
         <v>76</v>
       </c>
@@ -4910,7 +4928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="23" t="s">
         <v>76</v>
       </c>
@@ -4927,7 +4945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="23" t="s">
         <v>76</v>
       </c>
@@ -4947,7 +4965,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E89" s="29">
         <v>2</v>
       </c>
@@ -4955,7 +4973,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E90" s="29">
         <v>3</v>
       </c>
@@ -4963,7 +4981,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E91" s="29">
         <v>4</v>
       </c>
@@ -4971,7 +4989,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E92" s="29">
         <v>5</v>
       </c>
@@ -4979,7 +4997,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" s="23" t="s">
         <v>76</v>
       </c>
@@ -4999,7 +5017,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E94" s="29">
         <v>2</v>
       </c>
@@ -5007,7 +5025,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E95" s="29">
         <v>3</v>
       </c>
@@ -5015,7 +5033,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E96" s="29">
         <v>4</v>
       </c>
@@ -5023,7 +5041,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E97" s="29">
         <v>5</v>
       </c>
@@ -5031,7 +5049,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98" s="23" t="s">
         <v>76</v>
       </c>
@@ -5051,7 +5069,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E99" s="29">
         <v>2</v>
       </c>
@@ -5059,7 +5077,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E100" s="29">
         <v>3</v>
       </c>
@@ -5067,7 +5085,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E101" s="29">
         <v>4</v>
       </c>
@@ -5075,7 +5093,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102" s="23" t="s">
         <v>76</v>
       </c>
@@ -5095,7 +5113,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E103" s="29">
         <v>2</v>
       </c>
@@ -5103,7 +5121,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E104" s="29">
         <v>3</v>
       </c>
@@ -5111,7 +5129,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105" s="23" t="s">
         <v>76</v>
       </c>
@@ -5131,7 +5149,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E106" s="29">
         <v>2</v>
       </c>
@@ -5139,7 +5157,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E107" s="29">
         <v>3</v>
       </c>
@@ -5147,7 +5165,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E108" s="29">
         <v>4</v>
       </c>
@@ -5155,7 +5173,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109" s="23" t="s">
         <v>76</v>
       </c>
@@ -5175,7 +5193,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E110" s="29">
         <v>2</v>
       </c>
@@ -5183,7 +5201,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E111" s="29">
         <v>3</v>
       </c>
@@ -5191,7 +5209,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112" s="23" t="s">
         <v>76</v>
       </c>
@@ -5211,7 +5229,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="113" spans="1:14">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E113" s="29">
         <v>2</v>
       </c>
@@ -5219,7 +5237,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="114" spans="1:14">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E114" s="29">
         <v>3</v>
       </c>
@@ -5227,7 +5245,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="115" spans="1:14">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A115" s="23" t="s">
         <v>76</v>
       </c>
@@ -5247,7 +5265,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="116" spans="1:14">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E116" s="29">
         <v>2</v>
       </c>
@@ -5255,7 +5273,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="117" spans="1:14">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E117" s="29">
         <v>3</v>
       </c>
@@ -5266,7 +5284,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="118" spans="1:14">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E118" s="29">
         <v>4</v>
       </c>
@@ -5274,7 +5292,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="119" spans="1:14">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A119" s="23" t="s">
         <v>76</v>
       </c>
@@ -5291,7 +5309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:14">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A121" s="23" t="s">
         <v>76</v>
       </c>
@@ -5311,7 +5329,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="122" spans="1:14">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E122" s="29">
         <v>2</v>
       </c>
@@ -5319,7 +5337,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="123" spans="1:14">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E123" s="29">
         <v>3</v>
       </c>
@@ -5327,7 +5345,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="124" spans="1:14">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A124" s="23" t="s">
         <v>76</v>
       </c>
@@ -5347,17 +5365,17 @@
         <v>301</v>
       </c>
     </row>
-    <row r="125" spans="1:14">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G125" s="23" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="126" spans="1:14">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G126" s="23" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="127" spans="1:14">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A127" s="23" t="s">
         <v>76</v>
       </c>
@@ -5374,7 +5392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:14">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A128" s="23" t="s">
         <v>76</v>
       </c>
@@ -5391,7 +5409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A129" s="23" t="s">
         <v>76</v>
       </c>
@@ -5408,7 +5426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A130" s="23" t="s">
         <v>76</v>
       </c>
@@ -5425,7 +5443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A131" s="23" t="s">
         <v>76</v>
       </c>
@@ -5442,7 +5460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A132" s="23" t="s">
         <v>76</v>
       </c>
@@ -5459,7 +5477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A133" s="23" t="s">
         <v>76</v>
       </c>
@@ -5476,7 +5494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:5">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A134" s="23" t="s">
         <v>76</v>
       </c>
@@ -5493,7 +5511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:5">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A135" s="23" t="s">
         <v>76</v>
       </c>
@@ -5510,7 +5528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A136" s="23" t="s">
         <v>76</v>
       </c>
@@ -5527,7 +5545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A137" s="23" t="s">
         <v>76</v>
       </c>
@@ -5544,7 +5562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A138" s="23" t="s">
         <v>76</v>
       </c>
@@ -5560,55 +5578,71 @@
       <c r="E138" s="29">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:5">
-      <c r="A139" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="B139" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="C139" s="23" t="s">
+      <c r="G138" s="23" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G139" s="23" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G140" s="23" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A141" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B141" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C141" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="D139" s="23" t="s">
+      <c r="D141" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="E139" s="29">
+      <c r="E141" s="29">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:5">
-      <c r="A140" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="B140" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="C140" s="23" t="s">
+      <c r="G141" s="23" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A143" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B143" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C143" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="D140" s="23" t="s">
+      <c r="D143" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="E140" s="29">
+      <c r="E143" s="29">
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:5">
-      <c r="A141" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="B141" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="C141" s="23" t="s">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A144" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B144" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C144" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="D141" s="23" t="s">
+      <c r="D144" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="E141" s="29">
+      <c r="E144" s="29">
         <v>1</v>
       </c>
     </row>
@@ -5619,14 +5653,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
@@ -5637,7 +5671,7 @@
     <col min="9" max="9" width="4.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5">
+    <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>85</v>
       </c>
@@ -5666,7 +5700,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="16.5">
+    <row r="2" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
         <v>76</v>
       </c>
@@ -5687,7 +5721,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16.5">
+    <row r="3" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A3" s="23" t="s">
         <v>76</v>
       </c>
@@ -5706,7 +5740,7 @@
       <c r="H3" s="28"/>
       <c r="I3" s="28"/>
     </row>
-    <row r="4" spans="1:9" ht="16.5">
+    <row r="4" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A4" s="28"/>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
@@ -5717,7 +5751,7 @@
       <c r="H4" s="28"/>
       <c r="I4" s="28"/>
     </row>
-    <row r="5" spans="1:9" ht="16.5">
+    <row r="5" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A5" s="28"/>
       <c r="B5" s="28"/>
       <c r="C5" s="28"/>
@@ -5728,7 +5762,7 @@
       <c r="H5" s="28"/>
       <c r="I5" s="28"/>
     </row>
-    <row r="6" spans="1:9" ht="16.5">
+    <row r="6" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A6" s="28"/>
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
@@ -5739,7 +5773,7 @@
       <c r="H6" s="28"/>
       <c r="I6" s="28"/>
     </row>
-    <row r="7" spans="1:9" ht="16.5">
+    <row r="7" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A7" s="28"/>
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
@@ -5750,7 +5784,7 @@
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
     </row>
-    <row r="8" spans="1:9" ht="16.5">
+    <row r="8" spans="1:9" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A8" s="28"/>
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>

</xml_diff>